<commit_message>
shimin analysis updated for new masks
</commit_message>
<xml_diff>
--- a/Otsu+Morphology/patient_watershed_results.xlsx
+++ b/Otsu+Morphology/patient_watershed_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/kaiwen_liu_mail_utoronto_ca/Documents/Desktop/github_repo/heart_cardiac_mri_image_processing/Otsu+Morphology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_2F2132AAD310556AAB992011595ED87656CD9866" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6FB8A99-7F60-4091-9928-EE6BA197F569}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_5345D3AAD37056296F5A2D11595ED87656CD1888" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CBD04C1-D6C6-4A73-8058-C7ABE12A2199}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2115" yWindow="1965" windowWidth="26370" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="1965" windowWidth="26370" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="89">
   <si>
     <t>Patient ID</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>[88]</t>
+  </si>
+  <si>
+    <t>SCD0001901</t>
+  </si>
+  <si>
+    <t>[82]</t>
+  </si>
+  <si>
+    <t>SCD0002801</t>
   </si>
 </sst>
 </file>
@@ -640,18 +649,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1320,500 +1324,500 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
         <v>40</v>
       </c>
       <c r="E20">
-        <v>67.477942960409095</v>
+        <v>48.663902477659867</v>
       </c>
       <c r="F20">
-        <v>1492.452374686</v>
+        <v>439.96633892852589</v>
       </c>
       <c r="G20">
-        <v>485.37621258410968</v>
+        <v>225.86154881781749</v>
       </c>
       <c r="H20">
-        <v>571.81214266746724</v>
+        <v>286.69956380752649</v>
       </c>
       <c r="I20">
-        <v>371.36128214094271</v>
+        <v>194.25978046629959</v>
       </c>
       <c r="J20">
-        <v>141.78619668133891</v>
+        <v>94.364130551354179</v>
       </c>
       <c r="K20">
-        <v>97.50494060096932</v>
+        <v>75.558134450585143</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
         <v>40</v>
       </c>
       <c r="E21">
-        <v>76.289487160259227</v>
+        <v>67.477942960409095</v>
       </c>
       <c r="F21">
-        <v>445.61375559707921</v>
+        <v>1492.452374686</v>
       </c>
       <c r="G21">
-        <v>105.65730673649649</v>
+        <v>485.37621258410968</v>
       </c>
       <c r="H21">
-        <v>98.664434173967678</v>
+        <v>571.81214266746724</v>
       </c>
       <c r="I21">
-        <v>92.108277807538258</v>
+        <v>371.36128214094271</v>
       </c>
       <c r="J21">
-        <v>94.766168522656528</v>
+        <v>141.78619668133891</v>
       </c>
       <c r="K21">
-        <v>58.654360566084421</v>
+        <v>97.50494060096932</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
         <v>40</v>
       </c>
       <c r="E22">
-        <v>91.695690308523353</v>
+        <v>76.289487160259227</v>
       </c>
       <c r="F22">
-        <v>683.20710853637945</v>
+        <v>445.61375559707921</v>
       </c>
       <c r="G22">
-        <v>56.735634127043873</v>
+        <v>105.65730673649649</v>
       </c>
       <c r="H22">
-        <v>212.44301641870541</v>
+        <v>98.664434173967678</v>
       </c>
       <c r="I22">
-        <v>45.566453742420471</v>
+        <v>92.108277807538258</v>
       </c>
       <c r="J22">
-        <v>109.27427103980661</v>
+        <v>94.766168522656528</v>
       </c>
       <c r="K22">
-        <v>47.67445792372628</v>
+        <v>58.654360566084421</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
         <v>40</v>
       </c>
       <c r="E23">
-        <v>38.096240548554469</v>
+        <v>91.695690308523353</v>
       </c>
       <c r="F23">
-        <v>261.71266351087439</v>
+        <v>683.20710853637945</v>
       </c>
       <c r="G23">
-        <v>162.00997767374281</v>
+        <v>56.735634127043873</v>
       </c>
       <c r="H23">
-        <v>117.5660058817037</v>
+        <v>212.44301641870541</v>
       </c>
       <c r="I23">
-        <v>113.3577606235111</v>
+        <v>45.566453742420471</v>
       </c>
       <c r="J23">
-        <v>79.361287526318677</v>
+        <v>109.27427103980661</v>
       </c>
       <c r="K23">
-        <v>67.636487640333684</v>
+        <v>47.67445792372628</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
         <v>40</v>
       </c>
       <c r="E24">
-        <v>45.230720406375127</v>
+        <v>38.096240548554469</v>
       </c>
       <c r="F24">
-        <v>664.35772965388571</v>
+        <v>261.71266351087439</v>
       </c>
       <c r="G24">
-        <v>363.86394245599507</v>
+        <v>162.00997767374281</v>
       </c>
       <c r="H24">
-        <v>192.8806722017589</v>
+        <v>117.5660058817037</v>
       </c>
       <c r="I24">
-        <v>211.82986436417571</v>
+        <v>113.3577606235111</v>
       </c>
       <c r="J24">
-        <v>108.2599419775661</v>
+        <v>79.361287526318677</v>
       </c>
       <c r="K24">
-        <v>88.575470139826052</v>
+        <v>67.636487640333684</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E25">
-        <v>70.6447382201262</v>
+        <v>45.230720406375127</v>
       </c>
       <c r="F25">
-        <v>1259.4564097850671</v>
+        <v>664.35772965388571</v>
       </c>
       <c r="G25">
-        <v>369.71672609580662</v>
+        <v>363.86394245599507</v>
       </c>
       <c r="H25">
-        <v>344.30649825104229</v>
+        <v>192.8806722017589</v>
       </c>
       <c r="I25">
-        <v>116.7171756768338</v>
+        <v>211.82986436417571</v>
       </c>
       <c r="J25">
-        <v>133.98664303473191</v>
+        <v>108.2599419775661</v>
       </c>
       <c r="K25">
-        <v>89.047861057164226</v>
+        <v>88.575470139826052</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
         <v>58</v>
       </c>
       <c r="E26">
-        <v>85.557770134984509</v>
+        <v>70.6447382201262</v>
       </c>
       <c r="F26">
-        <v>228.74909867196291</v>
+        <v>1259.4564097850671</v>
       </c>
       <c r="G26">
-        <v>33.036470644355958</v>
+        <v>369.71672609580662</v>
       </c>
       <c r="H26">
-        <v>69.57900007823676</v>
+        <v>344.30649825104229</v>
       </c>
       <c r="I26">
-        <v>29.036584641498759</v>
+        <v>116.7171756768338</v>
       </c>
       <c r="J26">
-        <v>75.878765469667528</v>
+        <v>133.98664303473191</v>
       </c>
       <c r="K26">
-        <v>39.810564955411962</v>
+        <v>89.047861057164226</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
         <v>58</v>
       </c>
       <c r="E27">
-        <v>51.636509170254037</v>
+        <v>85.557770134984509</v>
       </c>
       <c r="F27">
-        <v>1217.3700404685419</v>
+        <v>228.74909867196291</v>
       </c>
       <c r="G27">
-        <v>588.76264788607784</v>
+        <v>33.036470644355958</v>
       </c>
       <c r="H27">
-        <v>121.1443426558302</v>
+        <v>69.57900007823676</v>
       </c>
       <c r="I27">
-        <v>81.455242330536365</v>
+        <v>29.036584641498759</v>
       </c>
       <c r="J27">
-        <v>132.47725754964341</v>
+        <v>75.878765469667528</v>
       </c>
       <c r="K27">
-        <v>103.9873575801937</v>
+        <v>39.810564955411962</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
         <v>58</v>
       </c>
       <c r="E28">
-        <v>47.342351757140321</v>
+        <v>62.216281615416413</v>
       </c>
       <c r="F28">
-        <v>339.07616097574351</v>
+        <v>23.814340910517991</v>
       </c>
       <c r="G28">
-        <v>178.54953212199959</v>
+        <v>8.9979435047747973</v>
       </c>
       <c r="H28">
-        <v>51.570382154048389</v>
+        <v>35.624142095488523</v>
       </c>
       <c r="I28">
-        <v>68.690323445556658</v>
+        <v>21.415739085971879</v>
       </c>
       <c r="J28">
-        <v>86.516620159299521</v>
+        <v>35.695487263568623</v>
       </c>
       <c r="K28">
-        <v>69.86398674056548</v>
+        <v>25.805654589247681</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
         <v>58</v>
       </c>
       <c r="E29">
-        <v>41.694473051810853</v>
+        <v>51.636509170254037</v>
       </c>
       <c r="F29">
-        <v>83.755171769146997</v>
+        <v>1217.3700404685419</v>
       </c>
       <c r="G29">
-        <v>48.833894246362107</v>
+        <v>588.76264788607784</v>
       </c>
       <c r="H29">
-        <v>62.710562998666873</v>
+        <v>121.1443426558302</v>
       </c>
       <c r="I29">
-        <v>30.373455772294601</v>
+        <v>81.455242330536365</v>
       </c>
       <c r="J29">
-        <v>54.283895249522331</v>
+        <v>132.47725754964341</v>
       </c>
       <c r="K29">
-        <v>45.349681926404493</v>
+        <v>103.9873575801937</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
         <v>58</v>
       </c>
       <c r="E30">
-        <v>37.658796911087762</v>
+        <v>47.342351757140321</v>
       </c>
       <c r="F30">
-        <v>2261.6985047907842</v>
+        <v>339.07616097574351</v>
       </c>
       <c r="G30">
-        <v>1409.970058130514</v>
+        <v>178.54953212199959</v>
       </c>
       <c r="H30">
-        <v>303.17566359357829</v>
+        <v>51.570382154048389</v>
       </c>
       <c r="I30">
-        <v>268.08570305205342</v>
+        <v>68.690323445556658</v>
       </c>
       <c r="J30">
-        <v>162.85909965973289</v>
+        <v>86.516620159299521</v>
       </c>
       <c r="K30">
-        <v>139.124544660943</v>
+        <v>69.86398674056548</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
         <v>58</v>
       </c>
       <c r="E31">
-        <v>84.890270395822824</v>
+        <v>41.694473051810853</v>
       </c>
       <c r="F31">
-        <v>89.276407493917674</v>
+        <v>83.755171769146997</v>
       </c>
       <c r="G31">
-        <v>13.48942377265432</v>
+        <v>48.833894246362107</v>
       </c>
       <c r="H31">
-        <v>44.830651106899971</v>
+        <v>62.710562998666873</v>
       </c>
       <c r="I31">
-        <v>32.003917907161501</v>
+        <v>30.373455772294601</v>
       </c>
       <c r="J31">
-        <v>55.451422868058778</v>
+        <v>54.283895249522331</v>
       </c>
       <c r="K31">
-        <v>29.534633908487351</v>
+        <v>45.349681926404493</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
         <v>58</v>
       </c>
       <c r="E32">
-        <v>84.989313102083884</v>
+        <v>37.658796911087762</v>
       </c>
       <c r="F32">
-        <v>406.84623770064809</v>
+        <v>2261.6985047907842</v>
       </c>
       <c r="G32">
-        <v>61.070414897195867</v>
+        <v>1409.970058130514</v>
       </c>
       <c r="H32">
-        <v>109.06553044863939</v>
+        <v>303.17566359357829</v>
       </c>
       <c r="I32">
-        <v>38.211599575683337</v>
+        <v>268.08570305205342</v>
       </c>
       <c r="J32">
-        <v>91.934226684535005</v>
+        <v>162.85909965973289</v>
       </c>
       <c r="K32">
-        <v>48.858944731180863</v>
+        <v>139.124544660943</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>58</v>
       </c>
       <c r="E33">
-        <v>89.342134588265409</v>
+        <v>84.890270395822824</v>
       </c>
       <c r="F33">
-        <v>138.79508940052321</v>
+        <v>89.276407493917674</v>
       </c>
       <c r="G33">
-        <v>14.792593826404451</v>
+        <v>13.48942377265432</v>
       </c>
       <c r="H33">
-        <v>73.887478226737485</v>
+        <v>44.830651106899971</v>
       </c>
       <c r="I33">
-        <v>35.526158133111998</v>
+        <v>32.003917907161501</v>
       </c>
       <c r="J33">
-        <v>64.237972658990643</v>
+        <v>55.451422868058778</v>
       </c>
       <c r="K33">
-        <v>30.45663393306021</v>
+        <v>29.534633908487351</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
         <v>47</v>
@@ -1822,340 +1826,410 @@
         <v>58</v>
       </c>
       <c r="E34">
-        <v>16.43309734471886</v>
+        <v>84.989313102083884</v>
       </c>
       <c r="F34">
-        <v>1190.650127546653</v>
+        <v>406.84623770064809</v>
       </c>
       <c r="G34">
-        <v>994.98943305189266</v>
+        <v>61.070414897195867</v>
       </c>
       <c r="H34">
-        <v>432.87723234443467</v>
+        <v>109.06553044863939</v>
       </c>
       <c r="I34">
-        <v>324.83807467847129</v>
+        <v>38.211599575683337</v>
       </c>
       <c r="J34">
-        <v>131.50083590874311</v>
+        <v>91.934226684535005</v>
       </c>
       <c r="K34">
-        <v>123.8625306047591</v>
+        <v>48.858944731180863</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E35">
-        <v>91.563096573699042</v>
+        <v>89.342134588265409</v>
       </c>
       <c r="F35">
-        <v>741.84642640162713</v>
+        <v>138.79508940052321</v>
       </c>
       <c r="G35">
-        <v>62.588866566970111</v>
+        <v>14.792593826404451</v>
       </c>
       <c r="H35">
-        <v>507.77382885710091</v>
+        <v>73.887478226737485</v>
       </c>
       <c r="I35">
-        <v>83.721453314588302</v>
+        <v>35.526158133111998</v>
       </c>
       <c r="J35">
-        <v>112.3151812297756</v>
+        <v>64.237972658990643</v>
       </c>
       <c r="K35">
-        <v>49.260576283049218</v>
+        <v>30.45663393306021</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E36">
-        <v>86.618424007386082</v>
+        <v>16.43309734471886</v>
       </c>
       <c r="F36">
-        <v>1040.405452242527</v>
+        <v>1190.650127546653</v>
       </c>
       <c r="G36">
-        <v>139.22264622313219</v>
+        <v>994.98943305189266</v>
       </c>
       <c r="H36">
-        <v>140.03070225322469</v>
+        <v>432.87723234443467</v>
       </c>
       <c r="I36">
-        <v>52.43313929901791</v>
+        <v>324.83807467847129</v>
       </c>
       <c r="J36">
-        <v>125.71911999068639</v>
+        <v>131.50083590874311</v>
       </c>
       <c r="K36">
-        <v>64.30386651131117</v>
+        <v>123.8625306047591</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
         <v>72</v>
       </c>
       <c r="E37">
-        <v>99.964692885462043</v>
+        <v>91.563096573699042</v>
       </c>
       <c r="F37">
-        <v>211.89725429713039</v>
+        <v>741.84642640162713</v>
       </c>
       <c r="G37">
-        <v>7.4814806277463966E-2</v>
+        <v>62.588866566970111</v>
       </c>
       <c r="H37">
-        <v>162.5143922764378</v>
+        <v>507.77382885710091</v>
       </c>
       <c r="I37">
-        <v>0.7045657734888815</v>
+        <v>83.721453314588302</v>
       </c>
       <c r="J37">
-        <v>73.967720605462048</v>
+        <v>112.3151812297756</v>
       </c>
       <c r="K37">
-        <v>5.2279285622564746</v>
+        <v>49.260576283049218</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
         <v>72</v>
       </c>
       <c r="E38">
-        <v>1.1600301411551299</v>
+        <v>86.618424007386082</v>
       </c>
       <c r="F38">
-        <v>3962.0542311588761</v>
+        <v>1040.405452242527</v>
       </c>
       <c r="G38">
-        <v>3916.09320786852</v>
+        <v>139.22264622313219</v>
       </c>
       <c r="H38">
-        <v>1643.1213828725461</v>
+        <v>140.03070225322469</v>
       </c>
       <c r="I38">
-        <v>1627.055614699135</v>
+        <v>52.43313929901791</v>
       </c>
       <c r="J38">
-        <v>196.32424281303031</v>
+        <v>125.71911999068639</v>
       </c>
       <c r="K38">
-        <v>195.56214819939331</v>
+        <v>64.30386651131117</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
         <v>72</v>
       </c>
       <c r="E39">
-        <v>2.3095127736262211</v>
+        <v>99.645193235415647</v>
       </c>
       <c r="F39">
-        <v>4735.3176133046554</v>
+        <v>327.48010283766888</v>
       </c>
       <c r="G39">
-        <v>4625.9548481536112</v>
+        <v>1.161921557535849</v>
       </c>
       <c r="H39">
-        <v>2931.4411096866502</v>
+        <v>138.40896485848251</v>
       </c>
       <c r="I39">
-        <v>2625.3556411110098</v>
+        <v>4.8833024646105274</v>
       </c>
       <c r="J39">
-        <v>208.34519897052559</v>
+        <v>85.518898530757795</v>
       </c>
       <c r="K39">
-        <v>206.72877082441309</v>
+        <v>13.043457547438869</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
         <v>72</v>
       </c>
       <c r="E40">
-        <v>5.9425229620809557</v>
+        <v>88.768188083646564</v>
       </c>
       <c r="F40">
-        <v>2688.970876301169</v>
+        <v>129.45133676634359</v>
       </c>
       <c r="G40">
-        <v>2529.1781645333022</v>
+        <v>14.539730668801001</v>
       </c>
       <c r="H40">
-        <v>1468.2774745900881</v>
+        <v>110.6090693469917</v>
       </c>
       <c r="I40">
-        <v>1469.9756219598321</v>
+        <v>33.455084304880103</v>
       </c>
       <c r="J40">
-        <v>172.52915372572289</v>
+        <v>62.762847515452712</v>
       </c>
       <c r="K40">
-        <v>169.041602238325</v>
+        <v>30.282094692666931</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
         <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
         <v>72</v>
       </c>
       <c r="E41">
-        <v>2.8186289730177498</v>
+        <v>80.371565191365548</v>
       </c>
       <c r="F41">
-        <v>4976.2955252468737</v>
+        <v>385.23622964182158</v>
       </c>
       <c r="G41">
-        <v>4836.0322177892785</v>
+        <v>75.615842194486262</v>
       </c>
       <c r="H41">
-        <v>2432.5289764633089</v>
+        <v>167.1169828908881</v>
       </c>
       <c r="I41">
-        <v>2393.9033865182619</v>
+        <v>96.636637343042665</v>
       </c>
       <c r="J41">
-        <v>211.8210811949975</v>
+        <v>90.276802222286193</v>
       </c>
       <c r="K41">
-        <v>209.8119343411152</v>
+        <v>52.465206967849213</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
         <v>72</v>
       </c>
       <c r="E42">
-        <v>1.2233277363177559</v>
+        <v>42.203279639091683</v>
       </c>
       <c r="F42">
-        <v>3933.8031352102912</v>
+        <v>280.77503494574171</v>
       </c>
       <c r="G42">
-        <v>3885.6798303651258</v>
+        <v>162.2787617908329</v>
       </c>
       <c r="H42">
-        <v>1923.2067461272891</v>
+        <v>140.75309610808799</v>
       </c>
       <c r="I42">
-        <v>1700.9791291842109</v>
+        <v>101.57837269263329</v>
       </c>
       <c r="J42">
-        <v>195.85650479792019</v>
+        <v>81.243125458649075</v>
       </c>
       <c r="K42">
-        <v>195.0545701079902</v>
+        <v>67.673871282679983</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
         <v>72</v>
       </c>
       <c r="E43">
-        <v>1.7421817029662889</v>
+        <v>56.915637673840052</v>
       </c>
       <c r="F43">
-        <v>5961.9651752234522</v>
+        <v>149.8246985651345</v>
       </c>
       <c r="G43">
-        <v>5858.0969088034872</v>
+        <v>64.551015983879509</v>
       </c>
       <c r="H43">
-        <v>2175.8977278345478</v>
+        <v>85.425992985509481</v>
       </c>
       <c r="I43">
-        <v>2024.70103153688</v>
+        <v>70.199214055877277</v>
       </c>
       <c r="J43">
-        <v>224.97293329154181</v>
+        <v>65.896385973181893</v>
       </c>
       <c r="K43">
-        <v>223.65879282047999</v>
+        <v>49.770058735355143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44">
+        <v>48.024511185456589</v>
+      </c>
+      <c r="F44">
+        <v>216.98050176483031</v>
+      </c>
+      <c r="G44">
+        <v>112.77667642451949</v>
+      </c>
+      <c r="H44">
+        <v>178.51813298324859</v>
+      </c>
+      <c r="I44">
+        <v>162.07577587448719</v>
+      </c>
+      <c r="J44">
+        <v>74.554528667694157</v>
+      </c>
+      <c r="K44">
+        <v>59.943241345001432</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45">
+        <v>68.570848664704869</v>
+      </c>
+      <c r="F45">
+        <v>331.93599701458578</v>
+      </c>
+      <c r="G45">
+        <v>104.3246668380349</v>
+      </c>
+      <c r="H45">
+        <v>140.45553625252811</v>
+      </c>
+      <c r="I45">
+        <v>85.014379455205216</v>
+      </c>
+      <c r="J45">
+        <v>85.905026604051642</v>
+      </c>
+      <c r="K45">
+        <v>58.406716889067027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>